<commit_message>
record linkcage EU OFAC v2
</commit_message>
<xml_diff>
--- a/record-linkage-of-ofac-and-eu-sanctions-lists/stats/comparisons.xlsx
+++ b/record-linkage-of-ofac-and-eu-sanctions-lists/stats/comparisons.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
-  <fileVersion appName="Calc"/>
+  <fileVersion appName="Calc" lowestEdited="4"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t xml:space="preserve">comparison_type</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
+  <si>
+    <t xml:space="preserve">comparison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type</t>
   </si>
   <si>
     <t xml:space="preserve">num_total_EU</t>
@@ -49,16 +52,28 @@
     <t xml:space="preserve">comp_num_na</t>
   </si>
   <si>
-    <t xml:space="preserve">Full</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Individuals_YOB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Companies_Country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Companies_Country_City</t>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type + Year of birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type + Address country ISO code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type + Address normalized city + country ISO code</t>
   </si>
 </sst>
 </file>
@@ -182,34 +197,34 @@
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1f497d"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="eeece1"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4f81bd"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="c0504d"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9bbb59"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064a2"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4bacc6"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="f79646"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ff"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
         <a:srgbClr val="800080"/>
@@ -354,23 +369,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -401,33 +417,39 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>28238</v>
+        <v>10</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>28238</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>34892</v>
+        <v>0</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>34892</v>
+        <v>344</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>0</v>
+        <v>344</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>488082452</v>
+        <v>0</v>
       </c>
       <c r="I2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -435,87 +457,480 @@
       <c r="A3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>17471</v>
+      <c r="B3" s="0" t="s">
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>15715</v>
+        <v>15835</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>1756</v>
+        <v>15835</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>18065</v>
+        <v>0</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>17355</v>
+        <v>16118</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>710</v>
+        <v>16118</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>6351522</v>
+        <v>0</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>42879790</v>
+        <v>255228530</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>12809</v>
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>8836</v>
+        <v>12403</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>3973</v>
+        <v>12403</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>22262</v>
+        <v>0</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>21776</v>
+        <v>18774</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>486</v>
+        <v>18774</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>31805603</v>
+        <v>0</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>92741222</v>
+        <v>232853922</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>1651</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>1651</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>344</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>344</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="C7" s="2" t="n">
+        <v>17471</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>15715</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>1756</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>18065</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>17355</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>710</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>6351522</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>42879790</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>12403</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>12403</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>18774</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>18774</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>232853922</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>1651</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>1651</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>344</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>343</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>16193</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>2735</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>13458</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>17609</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>14196</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>3413</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>1320925</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>246316477</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>12809</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>8836</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>3973</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>22262</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>21776</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>486</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>31805603</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>92741222</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>1651</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>1651</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>344</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>343</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>16583</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>2011</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>14572</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>19158</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>8867</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>10291</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>133558</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>299865577</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="2" t="n">
         <v>13986</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="D16" s="2" t="n">
         <v>8987</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="E16" s="2" t="n">
         <v>4999</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="F16" s="2" t="n">
         <v>27152</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="G16" s="2" t="n">
         <v>23137</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="H16" s="2" t="n">
         <v>4015</v>
       </c>
-      <c r="H5" s="2" t="n">
+      <c r="I16" s="2" t="n">
         <v>8065639</v>
       </c>
-      <c r="I5" s="2" t="n">
+      <c r="J16" s="2" t="n">
         <v>171815653</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>1651</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>1651</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
record linkage EU and OFAC v4
</commit_message>
<xml_diff>
--- a/record-linkage-of-ofac-and-eu-sanctions-lists/stats/comparisons.xlsx
+++ b/record-linkage-of-ofac-and-eu-sanctions-lists/stats/comparisons.xlsx
@@ -164,16 +164,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -372,564 +376,564 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2" t="n">
+      <c r="C2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="n">
         <v>344</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="3" t="n">
         <v>344</v>
       </c>
-      <c r="H2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2" t="n">
+      <c r="H2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="3" t="n">
         <v>15835</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="3" t="n">
         <v>15835</v>
       </c>
-      <c r="E3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="n">
+      <c r="E3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="n">
         <v>16118</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="3" t="n">
         <v>16118</v>
       </c>
-      <c r="H3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2" t="n">
+      <c r="H3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3" t="n">
         <v>255228530</v>
       </c>
-      <c r="J3" s="2" t="n">
+      <c r="J3" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="3" t="n">
         <v>12403</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="3" t="n">
         <v>12403</v>
       </c>
-      <c r="E4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2" t="n">
+      <c r="E4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3" t="n">
         <v>18774</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="3" t="n">
         <v>18774</v>
       </c>
-      <c r="H4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2" t="n">
+      <c r="H4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3" t="n">
         <v>232853922</v>
       </c>
-      <c r="J4" s="2" t="n">
+      <c r="J4" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2" t="n">
+      <c r="C5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="n">
         <v>1651</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="3" t="n">
         <v>1651</v>
       </c>
-      <c r="H5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2" t="n">
+      <c r="H5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="n">
+      <c r="C6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="n">
         <v>344</v>
       </c>
-      <c r="G6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2" t="n">
+      <c r="G6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3" t="n">
         <v>344</v>
       </c>
-      <c r="I6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2" t="n">
+      <c r="I6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="3" t="n">
         <v>17471</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="3" t="n">
         <v>15715</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="3" t="n">
         <v>1756</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="3" t="n">
         <v>18065</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G7" s="3" t="n">
         <v>17355</v>
       </c>
-      <c r="H7" s="2" t="n">
+      <c r="H7" s="3" t="n">
         <v>710</v>
       </c>
-      <c r="I7" s="2" t="n">
+      <c r="I7" s="3" t="n">
         <v>6351522</v>
       </c>
-      <c r="J7" s="2" t="n">
+      <c r="J7" s="3" t="n">
         <v>42879790</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" s="3" t="n">
         <v>12403</v>
       </c>
-      <c r="D8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2" t="n">
+      <c r="D8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3" t="n">
         <v>12403</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="3" t="n">
         <v>18774</v>
       </c>
-      <c r="G8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2" t="n">
+      <c r="G8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3" t="n">
         <v>18774</v>
       </c>
-      <c r="I8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="2" t="n">
+      <c r="I8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3" t="n">
         <v>232853922</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2" t="n">
+      <c r="C9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="n">
         <v>1651</v>
       </c>
-      <c r="G9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2" t="n">
+      <c r="G9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="n">
         <v>1651</v>
       </c>
-      <c r="I9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="2" t="n">
+      <c r="I9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2" t="n">
+      <c r="C10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="n">
         <v>344</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="G10" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H10" s="2" t="n">
+      <c r="H10" s="3" t="n">
         <v>343</v>
       </c>
-      <c r="I10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2" t="n">
+      <c r="I10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="C11" s="3" t="n">
         <v>16193</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="D11" s="3" t="n">
         <v>2735</v>
       </c>
-      <c r="E11" s="2" t="n">
+      <c r="E11" s="3" t="n">
         <v>13458</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="3" t="n">
         <v>17609</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G11" s="3" t="n">
         <v>14196</v>
       </c>
-      <c r="H11" s="2" t="n">
+      <c r="H11" s="3" t="n">
         <v>3413</v>
       </c>
-      <c r="I11" s="2" t="n">
+      <c r="I11" s="3" t="n">
         <v>1320925</v>
       </c>
-      <c r="J11" s="2" t="n">
+      <c r="J11" s="3" t="n">
         <v>246316477</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="2" t="n">
+      <c r="C12" s="3" t="n">
         <v>12809</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="D12" s="3" t="n">
         <v>8836</v>
       </c>
-      <c r="E12" s="2" t="n">
+      <c r="E12" s="3" t="n">
         <v>3973</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="3" t="n">
         <v>22262</v>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="G12" s="3" t="n">
         <v>21776</v>
       </c>
-      <c r="H12" s="2" t="n">
+      <c r="H12" s="3" t="n">
         <v>486</v>
       </c>
-      <c r="I12" s="2" t="n">
+      <c r="I12" s="3" t="n">
         <v>31805603</v>
       </c>
-      <c r="J12" s="2" t="n">
+      <c r="J12" s="3" t="n">
         <v>92741222</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2" t="n">
+      <c r="C13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3" t="n">
         <v>1651</v>
       </c>
-      <c r="G13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="2" t="n">
+      <c r="G13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="3" t="n">
         <v>1651</v>
       </c>
-      <c r="I13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="2" t="n">
+      <c r="I13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2" t="n">
+      <c r="C14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3" t="n">
         <v>344</v>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="G14" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H14" s="2" t="n">
+      <c r="H14" s="3" t="n">
         <v>343</v>
       </c>
-      <c r="I14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2" t="n">
+      <c r="I14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2" t="n">
+      <c r="C15" s="3" t="n">
         <v>16583</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="D15" s="3" t="n">
         <v>2011</v>
       </c>
-      <c r="E15" s="2" t="n">
+      <c r="E15" s="3" t="n">
         <v>14572</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F15" s="3" t="n">
         <v>19158</v>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="G15" s="3" t="n">
         <v>8867</v>
       </c>
-      <c r="H15" s="2" t="n">
+      <c r="H15" s="3" t="n">
         <v>10291</v>
       </c>
-      <c r="I15" s="2" t="n">
+      <c r="I15" s="3" t="n">
         <v>133558</v>
       </c>
-      <c r="J15" s="2" t="n">
+      <c r="J15" s="3" t="n">
         <v>299865577</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2" t="n">
+      <c r="C16" s="3" t="n">
         <v>13986</v>
       </c>
-      <c r="D16" s="2" t="n">
+      <c r="D16" s="3" t="n">
         <v>8987</v>
       </c>
-      <c r="E16" s="2" t="n">
+      <c r="E16" s="3" t="n">
         <v>4999</v>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="F16" s="3" t="n">
         <v>27152</v>
       </c>
-      <c r="G16" s="2" t="n">
+      <c r="G16" s="3" t="n">
         <v>23137</v>
       </c>
-      <c r="H16" s="2" t="n">
+      <c r="H16" s="3" t="n">
         <v>4015</v>
       </c>
-      <c r="I16" s="2" t="n">
+      <c r="I16" s="3" t="n">
         <v>8065639</v>
       </c>
-      <c r="J16" s="2" t="n">
+      <c r="J16" s="3" t="n">
         <v>171815653</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2" t="n">
+      <c r="C17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3" t="n">
         <v>1651</v>
       </c>
-      <c r="G17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="2" t="n">
+      <c r="G17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3" t="n">
         <v>1651</v>
       </c>
-      <c r="I17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" s="2" t="n">
+      <c r="I17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" s="3" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>